<commit_message>
Email send bug fix
</commit_message>
<xml_diff>
--- a/list_user.xlsx
+++ b/list_user.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,17 +461,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>74577</t>
+          <t>93528</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Бовин Степан Евгеньевич</t>
+          <t>Ярослав Кузнецов</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2019-01-31 00:00:00</t>
+          <t>?</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -486,220 +486,20 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>85341</t>
+          <t>49666</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Бовин Андрей Евгеньевич</t>
+          <t>Чернов Егор</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2014-12-31 00:00:00</t>
+          <t>?</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
-        <is>
-          <t>12345678</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>26319</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Мальчугина Елена Романовна</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2016-07-23 00:00:00</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>12345678</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>55128</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Низамеева Кристина Альбертовна</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2016-09-27 00:00:00</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>12345678</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>69483</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Низамеев Дамир Альбертович</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2014-06-25 00:00:00</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>12345678</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>18656</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Смирнов Матвей Александрович</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2017-04-17 00:00:00</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>12345678</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>28357</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Иванов Никита Борисович</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2017-03-23 00:00:00</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>12345678</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>36120</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Рогожина Мария Евгеньевна</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2016-05-10 00:00:00</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>12345678</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>93190</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Рогожин Александр Евгеньевич</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>2016-05-10 00:00:00</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>12345678</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>13180</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Макаревич Никита Валерьевич </t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>2015-12-29 00:00:00</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
         <is>
           <t>12345678</t>
         </is>

</xml_diff>